<commit_message>
Update to the Test table
</commit_message>
<xml_diff>
--- a/Teste de Mesa.xlsx
+++ b/Teste de Mesa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noite\Desktop\THEO\LP1-BD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab5314904be36c0d/0-Pastas/Banco de dados/LP1-BD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA11870-A50E-4ADF-9571-8A7132198729}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="163" documentId="13_ncr:1_{4CA11870-A50E-4ADF-9571-8A7132198729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43CA17FF-520C-4F3F-934D-746033006741}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9405" xr2:uid="{31C21C31-FBA6-47B3-815F-2AADA96E8363}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="11" xr2:uid="{31C21C31-FBA6-47B3-815F-2AADA96E8363}"/>
   </bookViews>
   <sheets>
     <sheet name="Exercício 1" sheetId="1" r:id="rId1"/>
@@ -19,26 +19,38 @@
     <sheet name="Exercício 4" sheetId="4" r:id="rId4"/>
     <sheet name="Exercício 5" sheetId="5" r:id="rId5"/>
     <sheet name="Exercício 6" sheetId="6" r:id="rId6"/>
-    <sheet name="Exercício 7" sheetId="7" r:id="rId7"/>
-    <sheet name=" Exercício 8" sheetId="8" r:id="rId8"/>
-    <sheet name="Exercício 9" sheetId="9" r:id="rId9"/>
-    <sheet name="Exercício 10" sheetId="10" r:id="rId10"/>
-    <sheet name="Exercício 11" sheetId="11" r:id="rId11"/>
-    <sheet name="Exercício 12" sheetId="12" r:id="rId12"/>
-    <sheet name="Exercício 13" sheetId="13" r:id="rId13"/>
-    <sheet name="Planilha13" sheetId="14" r:id="rId14"/>
+    <sheet name="Exercício 7-8" sheetId="7" r:id="rId7"/>
+    <sheet name="Exercício 9" sheetId="9" r:id="rId8"/>
+    <sheet name="Exercício 10" sheetId="10" r:id="rId9"/>
+    <sheet name="Exercício 11" sheetId="11" r:id="rId10"/>
+    <sheet name="Exercício 12-13" sheetId="12" r:id="rId11"/>
+    <sheet name="Exercício 14" sheetId="13" r:id="rId12"/>
+    <sheet name="Exercício 15" sheetId="14" r:id="rId13"/>
+    <sheet name="Exercício 16" sheetId="15" r:id="rId14"/>
+    <sheet name="Exercício 17" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
   <si>
     <t>c1</t>
   </si>
@@ -164,6 +176,63 @@
   </si>
   <si>
     <t>NÃO É POSITIVO</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c1 </t>
+  </si>
+  <si>
+    <t>Soma</t>
+  </si>
+  <si>
+    <t>Nota1</t>
+  </si>
+  <si>
+    <t>Nota2</t>
+  </si>
+  <si>
+    <t>Votar</t>
+  </si>
+  <si>
+    <t>AnoAtual</t>
+  </si>
+  <si>
+    <t>AnoNasc</t>
+  </si>
+  <si>
+    <t>Subtrair</t>
+  </si>
+  <si>
+    <t>Esse ano poderá votar</t>
+  </si>
+  <si>
+    <t>Esse ano não poderá votar</t>
+  </si>
+  <si>
+    <t>Valores</t>
+  </si>
+  <si>
+    <t>Num1</t>
+  </si>
+  <si>
+    <t>Num2</t>
+  </si>
+  <si>
+    <t>Resultado Maior</t>
+  </si>
+  <si>
+    <t>Ordem Crescente</t>
+  </si>
+  <si>
+    <t>Xadrez</t>
+  </si>
+  <si>
+    <t>Hora início</t>
+  </si>
+  <si>
+    <t>Hora fim</t>
   </si>
 </sst>
 </file>
@@ -210,7 +279,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -553,11 +622,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -575,45 +668,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -623,7 +715,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -633,16 +730,29 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,9 +771,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -701,7 +811,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -807,7 +917,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -949,7 +1059,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -959,7 +1069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BC3E682-6508-4AAE-AEE3-FC57E6689173}">
   <dimension ref="B1:X6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -986,11 +1096,8 @@
         <v>5</v>
       </c>
       <c r="E2" s="11"/>
-      <c r="O2" s="50"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="X2" s="26"/>
+      <c r="O2" s="27"/>
+      <c r="X2" s="20"/>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
@@ -1006,10 +1113,6 @@
         <f>PRODUCT(C3,D3)</f>
         <v>9125</v>
       </c>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="27"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
@@ -1045,12 +1148,12 @@
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="28">
         <f>SUM(E3:E5)</f>
         <v>9365</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1062,43 +1165,230 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3513194D-80C5-44F9-8F26-9EAA1C216770}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB3A414-1404-40FB-97C3-A2B8D8EE7247}">
+  <dimension ref="B1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2005</v>
+      </c>
+      <c r="D3" s="50" t="str">
+        <f>IMSUB(C4,C3)</f>
+        <v>19</v>
+      </c>
+      <c r="E3" s="34" t="str">
+        <f>IF(D3&gt;16,C5,C6)</f>
+        <v>Esse ano poderá votar</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2024</v>
+      </c>
+      <c r="D4" s="46"/>
+      <c r="E4" s="35"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="48"/>
+      <c r="C5" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="52"/>
+      <c r="E5" s="53"/>
+    </row>
+    <row r="6" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="26"/>
+      <c r="C6" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="29"/>
+      <c r="E6" s="30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="D3:D4"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB3A414-1404-40FB-97C3-A2B8D8EE7247}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CFAD295-C45F-49B6-82F2-5570E08C8F85}">
+  <dimension ref="B2:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <f>IF(C3&gt;C4,C3,C4)</f>
+        <v>999</v>
+      </c>
+      <c r="E3">
+        <f>IF(C3&gt;C4,C3,C4)</f>
+        <v>999</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4">
+        <v>999</v>
+      </c>
+      <c r="E4">
+        <f>IF(C3&gt;C4,C4,C3)</f>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CFAD295-C45F-49B6-82F2-5570E08C8F85}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17BFB2D3-7FB5-4C66-B65F-EDEEFF5F12C2}">
+  <dimension ref="B1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="6">
+        <v>15</v>
+      </c>
+      <c r="D3" s="31" t="str">
+        <f>IF(C3&lt;C4,B6,B7)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="14">
+        <v>13</v>
+      </c>
+      <c r="D4" s="33"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="45" t="str">
+        <f>IMSUB(C3,C4)</f>
+        <v>2</v>
+      </c>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="45" t="str">
+        <f>IMSUB(C4,C3)</f>
+        <v>-2</v>
+      </c>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="45" t="str">
+        <f>IMSUB(24,B5)</f>
+        <v>22</v>
+      </c>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="D3:D4"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17BFB2D3-7FB5-4C66-B65F-EDEEFF5F12C2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD33FF34-5718-425F-9D0E-CF29F8477E48}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1110,10 +1400,24 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD33FF34-5718-425F-9D0E-CF29F8477E48}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF4C68AD-9A30-4226-9A26-3DCF8D0DE71D}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{769DCBB4-3706-464D-8F9E-7DE6FF7C52FA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S29" sqref="S29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -1150,7 +1454,7 @@
       <c r="C3" s="6">
         <v>2000</v>
       </c>
-      <c r="D3" s="47">
+      <c r="D3" s="31">
         <f>SUM(C4:C6)</f>
         <v>989</v>
       </c>
@@ -1162,7 +1466,7 @@
       <c r="C4" s="2">
         <v>69</v>
       </c>
-      <c r="D4" s="48"/>
+      <c r="D4" s="32"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -1171,7 +1475,7 @@
       <c r="C5" s="2">
         <v>500</v>
       </c>
-      <c r="D5" s="48"/>
+      <c r="D5" s="32"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
@@ -1180,7 +1484,7 @@
       <c r="C6" s="2">
         <v>420</v>
       </c>
-      <c r="D6" s="48"/>
+      <c r="D6" s="32"/>
     </row>
     <row r="7" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
@@ -1190,7 +1494,7 @@
         <f>IMDIV(D3,C3)*100</f>
         <v>49.45</v>
       </c>
-      <c r="D7" s="49"/>
+      <c r="D7" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1229,7 +1533,7 @@
       <c r="C3" s="6">
         <v>1000</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="34">
         <f>PRODUCT(C3,C4)</f>
         <v>100</v>
       </c>
@@ -1241,7 +1545,7 @@
       <c r="C4" s="15">
         <v>0.1</v>
       </c>
-      <c r="D4" s="18"/>
+      <c r="D4" s="35"/>
     </row>
     <row r="5" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
@@ -1251,7 +1555,7 @@
         <f>SUM(C3:D3)</f>
         <v>1100</v>
       </c>
-      <c r="D5" s="19"/>
+      <c r="D5" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1276,10 +1580,10 @@
       <c r="B2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="17" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="11" t="s">
@@ -1287,16 +1591,16 @@
       </c>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="37">
+      <c r="C3" s="23">
         <v>1000</v>
       </c>
-      <c r="D3" s="38">
+      <c r="D3" s="24">
         <v>1.73</v>
       </c>
-      <c r="E3" s="39">
+      <c r="E3" s="25">
         <f>PRODUCT(C3,D3)</f>
         <v>1730</v>
       </c>
@@ -1321,24 +1625,24 @@
       <c r="B2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="16" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="6">
         <v>1500</v>
       </c>
-      <c r="D3" s="33">
+      <c r="D3" s="40">
         <v>0.05</v>
       </c>
       <c r="E3" s="12">
@@ -1347,13 +1651,13 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="2">
         <v>10</v>
       </c>
-      <c r="D4" s="30"/>
+      <c r="D4" s="41"/>
       <c r="E4" s="13">
         <f>PRODUCT(C4,C6)</f>
         <v>1000</v>
@@ -1366,7 +1670,7 @@
       <c r="C5" s="2">
         <v>3000</v>
       </c>
-      <c r="D5" s="30"/>
+      <c r="D5" s="41"/>
       <c r="E5" s="13">
         <f>PRODUCT(C4,E3)</f>
         <v>1500</v>
@@ -1379,19 +1683,19 @@
       <c r="C6" s="2">
         <v>100</v>
       </c>
-      <c r="D6" s="30"/>
+      <c r="D6" s="41"/>
       <c r="E6" s="13"/>
     </row>
     <row r="7" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="40">
+      <c r="C7" s="37">
         <f>SUM(E4,E5,C3)</f>
         <v>4000</v>
       </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="42"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1420,16 +1724,16 @@
       <c r="C2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="44"/>
+      <c r="E2" s="42"/>
       <c r="F2" s="16" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="6">
@@ -1449,7 +1753,7 @@
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C4" s="2">
@@ -1469,7 +1773,7 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="43"/>
+      <c r="B5" s="26"/>
       <c r="C5" s="2">
         <v>9</v>
       </c>
@@ -1558,11 +1862,11 @@
       <c r="C5" s="14">
         <v>-10</v>
       </c>
-      <c r="D5" s="28" t="str">
+      <c r="D5" s="21" t="str">
         <f>IF(C5&gt;10,D6,D7)</f>
         <v>O NÚMERO NÃO É MAIOR QUE 10</v>
       </c>
-      <c r="E5" s="29" t="str">
+      <c r="E5" s="22" t="str">
         <f>IF(C5&gt;0,D8,D9)</f>
         <v>NÃO É POSITIVO</v>
       </c>
@@ -1593,18 +1897,6 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A8D6C49-B29F-40A4-A762-75D05B7D2D91}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0580A4F9-EC0A-4B31-8E40-47EC72D2E016}">
   <dimension ref="B1:D4"/>
   <sheetViews>
@@ -1643,8 +1935,8 @@
         <f>PRODUCT(C3,1.3)</f>
         <v>6.5</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="46"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1652,4 +1944,67 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3513194D-80C5-44F9-8F26-9EAA1C216770}">
+  <dimension ref="B1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="6">
+        <v>7</v>
+      </c>
+      <c r="D3" s="50">
+        <f>SUM(C3:C4)</f>
+        <v>13</v>
+      </c>
+      <c r="E3" s="34" t="str">
+        <f>IMDIV(D3,2)</f>
+        <v>6,5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="14">
+        <v>6</v>
+      </c>
+      <c r="D4" s="47"/>
+      <c r="E4" s="36"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>